<commit_message>
Upload Sprint_info + Master_schedule
</commit_message>
<xml_diff>
--- a/Document/Sprint Info/FSA_FPT_Sprint1_Info_Group1.xlsx
+++ b/Document/Sprint Info/FSA_FPT_Sprint1_Info_Group1.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OJT\Doing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OJT\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167F7E34-B08E-4A81-BE62-E3CEFD995131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DE5E9F-7F3B-46C0-AD17-1C1E3306A718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="To do List" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="Sprint 01" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -36,7 +36,7 @@
     <definedName name="_e3" hidden="1">{"'表紙'!$A$1:$W$39"}</definedName>
     <definedName name="_e4" hidden="1">{"'表紙'!$A$1:$W$39"}</definedName>
     <definedName name="_e5" hidden="1">{"'表紙'!$A$1:$W$39"}</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint 01'!$A$17:$I$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint 01'!$A$17:$I$22</definedName>
     <definedName name="_hhh1" hidden="1">{"'フローチャート'!$A$1:$AO$191"}</definedName>
     <definedName name="_hhh2" hidden="1">{"'フローチャート'!$A$1:$AO$191"}</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="126">
   <si>
     <t>Planning - Forecast</t>
   </si>
@@ -515,9 +515,6 @@
     <t>(Forecast - Plan) AVG points/Member/Sprint</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -536,9 +533,6 @@
     <t>DueDate</t>
   </si>
   <si>
-    <t>Ticket Jira</t>
-  </si>
-  <si>
     <t>MinhNHL</t>
   </si>
   <si>
@@ -755,56 +749,113 @@
     <t>UC 54: Approve/ Reject create, edit course</t>
   </si>
   <si>
-    <t>Thiết kế mẫu cho các trang cần làm</t>
-  </si>
-  <si>
-    <t>Thiết kế database cho các dữ liệu liên quan ( Role: Admin, Instructor, Student )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đăng nhập với 2 hình thức ( tài khoản thuộc website, tài khoản bên thứ 3 ( facebook / gmail ) </t>
+    <t>User page</t>
   </si>
   <si>
     <t>Trang đăng ký bằng email ( tài khoản thuộc website ) với 2 role Instructor / Student</t>
   </si>
   <si>
-    <t>Chức năng quên mật khẩu với tài khoản thuộc website</t>
-  </si>
-  <si>
-    <t>Login Page</t>
-  </si>
-  <si>
     <t>In-progress</t>
   </si>
   <si>
-    <t>[Login Page] Design UI</t>
-  </si>
-  <si>
-    <t>[Login Page] Design Database</t>
-  </si>
-  <si>
-    <t>[Login Page] Login Page ( Login with gmail/facbook with verify )</t>
-  </si>
-  <si>
-    <t>[Login Page] Sign Up Page ( Instructor, Student )</t>
-  </si>
-  <si>
-    <t>[Login Page] Forgot password ( code xác thực bên thứ 3 )</t>
-  </si>
-  <si>
-    <t>Minh</t>
-  </si>
-  <si>
-    <t>Function</t>
+    <t>Basic Design</t>
+  </si>
+  <si>
+    <t>[Basic Design] Home Page</t>
+  </si>
+  <si>
+    <t>[Basic Design] Login</t>
+  </si>
+  <si>
+    <t>[Basic Design] Signup</t>
+  </si>
+  <si>
+    <t>[Basic Design] Infor Course</t>
+  </si>
+  <si>
+    <t>[Basic Design] Profile User</t>
+  </si>
+  <si>
+    <t>[Basic Design] Profile Instructor</t>
+  </si>
+  <si>
+    <t>[Basic Design] List Course</t>
+  </si>
+  <si>
+    <t>[Basic Design] Page Video Course</t>
+  </si>
+  <si>
+    <t>[Basic Design] Page Docs Course</t>
+  </si>
+  <si>
+    <t>[Basic Design] Page Quiz Course</t>
+  </si>
+  <si>
+    <t>[Basic Design] Admin Page</t>
+  </si>
+  <si>
+    <t>[Basic Design] Payment Page</t>
+  </si>
+  <si>
+    <t>[Basic Design] Course Management</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Khóa học Phờ Ri , Pro (Phải Mua)</t>
+  </si>
+  <si>
+    <t>06-Jun</t>
+  </si>
+  <si>
+    <t>Đăng nhập với 2 hình thức ( tài khoản thuộc website, tài khoản bên thứ 3 ( facebook / gmail )</t>
+  </si>
+  <si>
+    <t>Thông tin của khóa học ( Mô tả về khóa học , thời gian lượng khóa học , kĩ năng đạt được . etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduce User , Khóa học đã đăng ký , Instructor đã theo dõi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduce Instrucor, khóa học đã bán , Số lượng Student enroll </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter/Search khóa học theo từng loại ( BE , FE ) , Filter theo giá ( Thấp - Cao ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiện thị video nội dung của khóa học , thông tin của khóa học </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiện thị nôi dung của khóa học , tips , cách dùng / làm </t>
+  </si>
+  <si>
+    <t>Hiện thị câu hỏi ( Multiple Choice ) , Pass % , Review Quiz , Try Again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dash board , User Management ( CRUD) , Approve  (Category , Course ) </t>
+  </si>
+  <si>
+    <t>Tổng tiền khóa học , phương thức thanh toán ( VNPAY , Payment )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Basic Design] Edit Profile Page </t>
+  </si>
+  <si>
+    <t>Thay đổi họ tên , thay đổi người dùng hiện thị , đổi mật khẩu, thay đổi Introduce, đổi ảnh avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRUD </t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,15 +874,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -839,79 +882,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -919,7 +911,7 @@
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -927,7 +919,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -935,14 +927,14 @@
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -950,7 +942,7 @@
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -958,7 +950,7 @@
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -966,28 +958,28 @@
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -999,7 +991,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="128"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1007,28 +999,22 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri Light"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -1038,13 +1024,84 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1054,19 +1111,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,126 +1201,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1274,60 +1283,60 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FFED7D31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FFE2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor rgb="FFF8CBAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FFC6E0B4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="15">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1343,34 +1352,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1482,504 +1463,251 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="38" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="38">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="38" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="38" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="38" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="38" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="38" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="38" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="38" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="38" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="38" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="2" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="38" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="2" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="38" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="38" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="40" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="38" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="38" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="5" xfId="38" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="38" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="38" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="38" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="5" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="38" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="40" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="38" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="38" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="38" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="38" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="38" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="38" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="38" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="38" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="3" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="38" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="7" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="38" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="51">
-    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Bad 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Calculation 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Check Cell 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Good 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Heading 1 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Heading 2 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Heading 3 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Heading 4 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Input 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Neutral 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+  <cellStyles count="50">
+    <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Accent1 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Accent2 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Accent3 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Accent4 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Accent5 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Accent6 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Bad 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Calculation 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Check Cell 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Good 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Heading 1 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Heading 2 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Heading 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Heading 4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Input 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Neutral 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 4" xfId="43" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 7 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 8 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Note 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Output 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Title 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Total 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Warning Text 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 3 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 4" xfId="42" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 7 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 8 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Note 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Output 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Title 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Total 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Warning Text 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1997,24 +1725,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="F2:I8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PIC" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Point" dataDxfId="2">
-      <calculatedColumnFormula>SUMIF($H$18:$H$58,Table1[[#This Row],[PIC]],$J$18:$J$58)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Release Point" dataDxfId="1">
-      <calculatedColumnFormula>SUMIFS($I$18:$I$22,$G$18:$G$22,"DaiNT12",$F$18:$F$22,"Done (FPT side)")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Total ID" dataDxfId="0">
-      <calculatedColumnFormula>COUNTIF(G17:G22,Table1[[#This Row],[PIC]])</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2275,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851E835C-4DBA-4B16-B522-C5D3104D9126}">
-  <dimension ref="B1:D36"/>
+  <dimension ref="B1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2289,64 +1999,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="C1" s="31" t="s">
-        <v>107</v>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:4">
-      <c r="B2" s="30">
-        <v>1</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>30</v>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
-        <v>29</v>
+      <c r="D5" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="56"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" t="s">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="30">
-        <v>2</v>
-      </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2479,18 +2194,18 @@
       </c>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" t="s">
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="30">
-        <v>3</v>
-      </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2564,14 +2279,6 @@
       </c>
       <c r="C35" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2582,554 +2289,854 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="87.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="61" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="18">
-      <c r="B1" s="57" t="s">
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="3"/>
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="34"/>
-      <c r="G1" s="57" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-    </row>
-    <row r="2" spans="2:15" ht="15.6">
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="54" t="s">
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.6">
+      <c r="A2" s="3"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:15">
-      <c r="B3" s="6" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="14.4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="51" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" ht="14.4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" ht="14.4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="29">
-        <f>SUMIF($G$18:$G$22,Table1[[#This Row],[PIC]],$I$18:$I$22)</f>
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H3" s="29">
-        <f>SUMIFS($I$18:$I$22,$G$18:$G$22,Table1[[#This Row],[PIC]],$F$18:$F$22,"Done (FPT side)")</f>
+      <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="I3" s="52">
-        <f>COUNTIF(G17:G22,Table1[[#This Row],[PIC]])</f>
+      <c r="I5" s="14">
         <v>0</v>
       </c>
-      <c r="J3" s="38"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-    </row>
-    <row r="4" spans="2:15">
-      <c r="B4" s="6" t="s">
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" ht="14.4">
+      <c r="A6" s="3"/>
+      <c r="B6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0</v>
+      </c>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.4">
+      <c r="A7" s="3"/>
+      <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
+      <c r="C7" s="16">
+        <v>8</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="51" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="14.4">
+      <c r="A8" s="3"/>
+      <c r="B8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="14.4">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.4">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" ht="14.4">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" ht="14.4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" ht="14.4">
+      <c r="A16" s="3"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" ht="14.4">
+      <c r="A17" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" ht="14.4">
+      <c r="A18" s="34">
+        <v>1</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="36">
+        <v>1</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="35"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" ht="14.4">
+      <c r="A19" s="34">
+        <v>2</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="36">
+        <v>1</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="35"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" ht="14.4">
+      <c r="A20" s="34">
+        <v>3</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="36">
+        <v>1</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.6" customHeight="1">
+      <c r="A21" s="34">
+        <v>4</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="36">
+        <v>1</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="29">
-        <f>SUMIF($G$18:$G$22,Table1[[#This Row],[PIC]],$I$18:$I$22)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="29">
-        <f>SUMIFS($I$18:$I$22,$G$18:$G$22,Table1[[#This Row],[PIC]],$F$18:$F$22,"Done (FPT side)")</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="52">
-        <f>COUNTIF(G18:G22,Table1[[#This Row],[PIC]])</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-    </row>
-    <row r="5" spans="2:15">
-      <c r="B5" s="8" t="s">
+      <c r="H21" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" ht="14.4">
+      <c r="A22" s="34">
+        <v>5</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="36">
+        <v>1</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I22" s="35"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" ht="14.4">
+      <c r="A23" s="34">
+        <v>6</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="36">
+        <v>1</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I23" s="35"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" ht="14.4">
+      <c r="A24" s="34">
+        <v>7</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="36">
+        <v>1</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I24" s="35"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" ht="14.4">
+      <c r="A25" s="34">
+        <v>8</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="36">
+        <v>1</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" s="35"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" ht="14.4">
+      <c r="A26" s="34">
+        <v>9</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="36">
+        <v>1</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I26" s="35"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" ht="14.4">
+      <c r="A27" s="34">
         <v>10</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="51" t="s">
+      <c r="B27" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="36">
+        <v>1</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="29">
-        <f>SUMIF($G$18:$G$22,Table1[[#This Row],[PIC]],$I$18:$I$22)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="29">
-        <f>SUMIFS($I$18:$I$22,$G$18:$G$22,Table1[[#This Row],[PIC]],$F$18:$F$22,"Done (FPT side)")</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="52">
-        <f>COUNTIF(G18:G22,Table1[[#This Row],[PIC]])</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-    </row>
-    <row r="6" spans="2:15">
-      <c r="B6" s="11" t="s">
+      <c r="H27" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" s="35"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" ht="14.4">
+      <c r="A28" s="34">
         <v>11</v>
       </c>
-      <c r="C6" s="12">
-        <f>I16</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="29">
-        <f>SUMIF($G$18:$G$22,Table1[[#This Row],[PIC]],$I$18:$I$22)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="29">
-        <f>SUMIFS($I$18:$I$22,$G$18:$G$22,Table1[[#This Row],[PIC]],$F$18:$F$22,"Done (FPT side)")</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="52">
-        <f>COUNTIF(G18:G22,Table1[[#This Row],[PIC]])</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-    </row>
-    <row r="7" spans="2:15">
-      <c r="B7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9">
-        <v>8</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="29">
-        <f>SUMIF($G$18:$G$22,Table1[[#This Row],[PIC]],$I$18:$I$22)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="29">
-        <f>SUMIFS($I$18:$I$22,$G$18:$G$22,Table1[[#This Row],[PIC]],$F$18:$F$22,"Done (FPT side)")</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="52">
-        <f>COUNTIF(G19:G23,Table1[[#This Row],[PIC]])</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="42"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-    </row>
-    <row r="8" spans="2:15">
-      <c r="B8" s="13" t="s">
+      <c r="B28" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="36">
+        <v>1</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="35"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" ht="14.4">
+      <c r="A29" s="34">
+        <v>12</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="36">
+        <v>1</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" s="35"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" ht="14.4">
+      <c r="A30" s="34">
         <v>13</v>
       </c>
-      <c r="C8" s="14">
-        <f>C6/C7</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="45">
-        <f>SUM(G4:G7)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="46">
-        <f>SUM(H4:H7)</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="47">
-        <f>SUM(I4:I7)</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="43"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-    </row>
-    <row r="9" spans="2:15">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="39"/>
-    </row>
-    <row r="10" spans="2:15">
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="39"/>
-    </row>
-    <row r="11" spans="2:15">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-    </row>
-    <row r="12" spans="2:15">
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-    </row>
-    <row r="13" spans="2:15">
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-    </row>
-    <row r="14" spans="2:15">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:15">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:15">
-      <c r="C16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="G16" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="25">
-        <f>SUM(I18:I22)</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="26"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="19" t="s">
+      <c r="B30" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="36">
+        <v>1</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" s="39"/>
+    </row>
+    <row r="31" spans="1:14" ht="14.4">
+      <c r="A31" s="34">
         <v>14</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="21">
+      <c r="B31" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="36">
         <v>1</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="32" t="s">
+      <c r="F31" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="22">
-        <v>1</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" s="24">
-        <v>45449</v>
-      </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="21">
-        <v>2</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="22">
-        <v>1</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19" s="24">
-        <v>45449</v>
-      </c>
-      <c r="I19" s="26"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="21">
-        <v>3</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" s="22">
-        <v>1</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="24">
-        <v>45449</v>
-      </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.6" customHeight="1">
-      <c r="A21" s="21">
-        <v>4</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="22">
-        <v>1</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="24">
-        <v>45449</v>
-      </c>
-      <c r="I21" s="26"/>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="21">
-        <v>5</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="H22" s="24">
-        <v>45449</v>
-      </c>
-      <c r="I22" s="26"/>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="C23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="C24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="C25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="C26" s="2"/>
-      <c r="E26" s="1"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="F28" s="37"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="F29" s="37"/>
+      <c r="G31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="I31" s="39"/>
+    </row>
+    <row r="32" spans="1:14" ht="14.4">
+      <c r="G32" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A17:I17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A17:J22" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:J22">
+      <sortCondition ref="A17:A22"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="B1:D1"/>
@@ -3140,14 +3147,32 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="3fb232fd-8e72-43c7-b876-2e7a665041d4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3fb232fd-8e72-43c7-b876-2e7a665041d4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d6b8b58b-189a-48e8-8fd2-2265e728ba2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C2847DC6746C624DA076054CC14B56BE" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d1a86ca6fd1cf24b8780b905555cc29f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3fb232fd-8e72-43c7-b876-2e7a665041d4" xmlns:ns3="d6b8b58b-189a-48e8-8fd2-2265e728ba2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="664dce43fec14307dc8ce851907cad28" ns2:_="" ns3:_="">
     <xsd:import namespace="3fb232fd-8e72-43c7-b876-2e7a665041d4"/>
@@ -3382,29 +3407,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="3fb232fd-8e72-43c7-b876-2e7a665041d4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3fb232fd-8e72-43c7-b876-2e7a665041d4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d6b8b58b-189a-48e8-8fd2-2265e728ba2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36DBC693-E6D1-4B2F-B156-830E7F667C82}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9CCB141-5126-4675-81DE-8B8502A7672E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -3416,7 +3420,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9CCB141-5126-4675-81DE-8B8502A7672E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36DBC693-E6D1-4B2F-B156-830E7F667C82}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>